<commit_message>
ajustes en diseño y manual de instalación
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/diseño/reportes/mockups diseño reportes.xlsx
+++ b/documentacion/desarrollo/diseño/reportes/mockups diseño reportes.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pantalla de generacion reporte" sheetId="1" r:id="rId1"/>
     <sheet name="Informe de insidencia" sheetId="2" r:id="rId2"/>
+    <sheet name="Reporte visita técnica" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>ALCALDÍA DE SANTIAGO DE CALI</t>
   </si>
@@ -112,6 +113,18 @@
   </si>
   <si>
     <t>Invación</t>
+  </si>
+  <si>
+    <t>Calidad de bien</t>
+  </si>
+  <si>
+    <t>Tipo visi.</t>
+  </si>
+  <si>
+    <t>Uso público</t>
+  </si>
+  <si>
+    <t>Servicio P</t>
   </si>
 </sst>
 </file>
@@ -782,7 +795,7 @@
   <dimension ref="C1:AA23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:H3"/>
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1133,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -1420,4 +1432,291 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="0.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="9"/>
+      <c r="D7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="22">
+        <v>11222</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="22">
+        <v>11222</v>
+      </c>
+      <c r="I9" s="9">
+        <v>4565666662</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="22">
+        <v>11222</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="22">
+        <v>11222</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="22">
+        <v>11222</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
s agrega documentacion y apk del aplicativo movil
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/diseño/reportes/mockups diseño reportes.xlsx
+++ b/documentacion/desarrollo/diseño/reportes/mockups diseño reportes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Pantalla de generacion reporte" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>ALCALDÍA DE SANTIAGO DE CALI</t>
   </si>
@@ -125,13 +125,16 @@
   </si>
   <si>
     <t>Servicio P</t>
+  </si>
+  <si>
+    <t>terreno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +156,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -315,27 +324,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +458,7 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>152401</xdr:colOff>
+          <xdr:colOff>152400</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -794,8 +803,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="C1:AA23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +925,9 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
+      <c r="Z9" t="s">
+        <v>33</v>
+      </c>
       <c r="AA9" t="s">
         <v>9</v>
       </c>
@@ -935,11 +947,11 @@
     </row>
     <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="3:27" x14ac:dyDescent="0.25">
@@ -989,11 +1001,11 @@
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
@@ -1060,18 +1072,19 @@
       <formula1>$AA$6:$AA$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:H11">
-      <formula1>$Z$6:$Z$8</formula1>
+      <formula1>$Z$6:$Z$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId3" name="Button 3">
+            <control shapeId="1027" r:id="rId4" name="Button 3">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Buscar">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -1093,7 +1106,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId4" name="Button 5">
+            <control shapeId="1029" r:id="rId5" name="Button 5">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Buscar">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -1141,20 +1154,20 @@
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="13"/>
+      <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
@@ -1196,34 +1209,34 @@
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="9"/>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="16" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
-      <c r="D9" s="16">
+      <c r="D9" s="22">
         <v>20</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17">
+      <c r="E9" s="22"/>
+      <c r="F9" s="14">
         <v>3</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <v>4</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>13</v>
       </c>
       <c r="I9" s="9"/>
@@ -1259,19 +1272,19 @@
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="16" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="9"/>
@@ -1284,13 +1297,13 @@
       <c r="E14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="17">
         <v>43596</v>
       </c>
       <c r="G14" s="9">
         <v>4</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="18">
         <v>11222</v>
       </c>
       <c r="I14" s="9"/>
@@ -1303,13 +1316,13 @@
       <c r="E15" s="9">
         <v>4565666662</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="17">
         <v>43596</v>
       </c>
       <c r="G15" s="9">
         <v>4</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="18">
         <v>11222</v>
       </c>
       <c r="I15" s="9"/>
@@ -1322,13 +1335,13 @@
       <c r="E16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="17">
         <v>43596</v>
       </c>
       <c r="G16" s="9">
         <v>4</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="18">
         <v>11222</v>
       </c>
       <c r="I16" s="9"/>
@@ -1341,13 +1354,13 @@
       <c r="E17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="17">
         <v>43596</v>
       </c>
       <c r="G17" s="9">
         <v>4</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="18">
         <v>11222</v>
       </c>
       <c r="I17" s="9"/>
@@ -1360,13 +1373,13 @@
       <c r="E18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="17">
         <v>43596</v>
       </c>
       <c r="G18" s="9">
         <v>4</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="18">
         <v>11222</v>
       </c>
       <c r="I18" s="9"/>
@@ -1438,7 +1451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1457,20 +1470,20 @@
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="13"/>
+      <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
@@ -1501,19 +1514,19 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1525,10 +1538,10 @@
       <c r="F8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="18">
         <v>11222</v>
       </c>
       <c r="I8" s="9" t="s">
@@ -1543,10 +1556,10 @@
       <c r="F9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="18">
         <v>11222</v>
       </c>
       <c r="I9" s="9">
@@ -1561,10 +1574,10 @@
       <c r="F10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="18">
         <v>11222</v>
       </c>
       <c r="I10" s="9" t="s">
@@ -1579,10 +1592,10 @@
       <c r="F11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="18">
         <v>11222</v>
       </c>
       <c r="I11" s="9" t="s">
@@ -1598,10 +1611,10 @@
       <c r="F12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="18">
         <v>11222</v>
       </c>
       <c r="I12" s="9" t="s">

</xml_diff>